<commit_message>
Documentación y ajuste a BLP con caso de que no pueda leer
</commit_message>
<xml_diff>
--- a/BLPObl/docs/Test Parte 1.xlsx
+++ b/BLPObl/docs/Test Parte 1.xlsx
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12576" windowHeight="3660"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12576" windowHeight="3660" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Primera prueba" sheetId="1" r:id="rId1"/>
+    <sheet name="segunda prueba" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="37">
   <si>
     <t>write lyle lobj 10</t>
   </si>
@@ -112,6 +112,30 @@
   </si>
   <si>
     <t>NO EXISTE LUCAS</t>
+  </si>
+  <si>
+    <t>write hal hobj</t>
+  </si>
+  <si>
+    <t>read hal</t>
+  </si>
+  <si>
+    <t>write lyle hobj 20</t>
+  </si>
+  <si>
+    <t>foo lyle lobj</t>
+  </si>
+  <si>
+    <t>Hi lyle, This is hal</t>
+  </si>
+  <si>
+    <t>The missile launch code is 1234567</t>
+  </si>
+  <si>
+    <t>BAD_INSTRUCCION</t>
+  </si>
+  <si>
+    <t>PROBLEMA PERMISOS</t>
   </si>
 </sst>
 </file>
@@ -461,8 +485,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -550,7 +574,7 @@
         <v>26</v>
       </c>
       <c r="E5" s="2">
-        <v>20</v>
+        <v>0</v>
       </c>
       <c r="F5">
         <v>90</v>
@@ -736,5 +760,177 @@
     <mergeCell ref="G13:H13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="19.88671875" customWidth="1"/>
+    <col min="2" max="2" width="22.6640625" customWidth="1"/>
+    <col min="3" max="4" width="0" hidden="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="4"/>
+      <c r="G2" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" s="4"/>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="2">
+        <v>0</v>
+      </c>
+      <c r="F4" s="3">
+        <v>10</v>
+      </c>
+      <c r="G4" s="2">
+        <v>10</v>
+      </c>
+      <c r="H4" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>34</v>
+      </c>
+      <c r="B13" t="s">
+        <v>35</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="E1:H1"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>